<commit_message>
csv para xlxs com parametro
</commit_message>
<xml_diff>
--- a/teste_planilha.xlsx
+++ b/teste_planilha.xlsx
@@ -4,29 +4,48 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <charset val="1"/>
+      <family val="0"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,21 +69,45 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -167,7 +210,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>2</row>
+      <row>3</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -192,7 +235,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>3</row>
+      <row>4</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -217,7 +260,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>4</row>
+      <row>5</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -242,7 +285,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>5</row>
+      <row>6</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -267,7 +310,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>6</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -292,7 +335,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>7</row>
+      <row>8</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -317,7 +360,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>8</row>
+      <row>9</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -342,7 +385,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>10</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -367,7 +410,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>10</row>
+      <row>11</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -392,7 +435,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>11</row>
+      <row>12</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -417,7 +460,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>12</row>
+      <row>13</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -442,7 +485,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>13</row>
+      <row>14</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -467,7 +510,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>15</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -492,7 +535,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>15</row>
+      <row>16</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -517,7 +560,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>16</row>
+      <row>17</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -542,7 +585,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>17</row>
+      <row>18</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -567,7 +610,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>18</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -592,7 +635,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>19</row>
+      <row>20</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -617,7 +660,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>20</row>
+      <row>21</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -642,7 +685,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>21</row>
+      <row>22</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -667,7 +710,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>22</row>
+      <row>23</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -692,7 +735,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>23</row>
+      <row>24</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -717,7 +760,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>24</row>
+      <row>25</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -742,7 +785,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>25</row>
+      <row>26</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -767,7 +810,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>26</row>
+      <row>27</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="762000" cy="762000"/>
@@ -778,31 +821,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId26"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>27</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="762000" cy="762000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="27" name="Image 27" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -817,41 +835,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -859,1601 +877,1498 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="7" customWidth="1" min="4" max="4"/>
-    <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="7" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="42" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="14" customWidth="1" min="10" max="10"/>
-    <col width="9" customWidth="1" min="11" max="11"/>
-    <col width="7" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
-    <col width="7" customWidth="1" min="14" max="14"/>
-    <col width="13" customWidth="1" min="15" max="15"/>
-    <col width="9" customWidth="1" min="16" max="16"/>
-    <col width="17" customWidth="1" min="17" max="17"/>
-    <col width="18" customWidth="1" min="18" max="18"/>
-    <col width="14" customWidth="1" min="19" max="19"/>
-    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" style="3" min="1" max="1"/>
+    <col width="9" customWidth="1" style="3" min="2" max="2"/>
+    <col width="12" customWidth="1" style="3" min="3" max="3"/>
+    <col width="7" customWidth="1" style="3" min="4" max="4"/>
+    <col width="8" customWidth="1" style="3" min="5" max="5"/>
+    <col width="7" customWidth="1" style="3" min="6" max="6"/>
+    <col width="17" customWidth="1" style="3" min="7" max="7"/>
+    <col width="42" customWidth="1" style="3" min="8" max="8"/>
+    <col width="14" customWidth="1" style="3" min="9" max="10"/>
+    <col width="9" customWidth="1" style="3" min="11" max="11"/>
+    <col width="7" customWidth="1" style="3" min="12" max="12"/>
+    <col width="11" customWidth="1" style="3" min="13" max="13"/>
+    <col width="7" customWidth="1" style="3" min="14" max="14"/>
+    <col width="13" customWidth="1" style="3" min="15" max="15"/>
+    <col width="9" customWidth="1" style="3" min="16" max="16"/>
+    <col width="17" customWidth="1" style="3" min="17" max="17"/>
+    <col width="18" customWidth="1" style="3" min="18" max="18"/>
+    <col width="14" customWidth="1" style="3" min="19" max="19"/>
+    <col width="10" customWidth="1" style="3" min="20" max="20"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>FOTO</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>REMESSA</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>ENTREGA</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>TALAO</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>MODELO</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>PARES</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>CAMPO</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>MATERIAL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>CONSUMO</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>SALDO</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>UNIDADE</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Almox</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>Corte Maq</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>Corte</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="5" t="inlineStr">
         <is>
           <t>Pre-costura</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>Costura</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="5" t="inlineStr">
         <is>
           <t>Revisao Costura</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="5" t="inlineStr">
         <is>
           <t>Pre Cont.Interno</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="5" t="inlineStr">
         <is>
           <t>Distribuicao</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="5" t="inlineStr">
         <is>
           <t>Montagem</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="68" customHeight="1">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+    <row r="2" ht="68" customHeight="1" s="4">
+      <c r="A2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">CABEDAL        </t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC CEREJA - TB                    </t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,8288</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0000</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="68" customHeight="1">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+    <row r="3" ht="15" customHeight="1" s="4">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">./IMAGENS/0131291.BMP                        </t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="E3" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">COST. PALMILHA </t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NA COR                                  </t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0007</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0000</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="68" customHeight="1">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+    <row r="4" ht="68" customHeight="1" s="4">
+      <c r="A4" s="3" t="inlineStr"/>
+      <c r="B4" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO          </t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC CEREJA - TB                    </t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1556</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0000</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="68" customHeight="1">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+    <row r="5" ht="68" customHeight="1" s="4">
+      <c r="A5" s="3" t="inlineStr"/>
+      <c r="B5" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="E5" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO         </t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO SINT ROSADO                      </t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1301</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    256,6400</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="68" customHeight="1">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+    <row r="6" ht="68" customHeight="1" s="4">
+      <c r="A6" s="3" t="inlineStr"/>
+      <c r="B6" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="E6" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">FORRO SILK     </t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SILK ROSADO                             </t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,3889</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    196,8900</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K6" s="3" t="inlineStr">
         <is>
           <t>ML.</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="68" customHeight="1">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+    <row r="7" ht="68" customHeight="1" s="4">
+      <c r="A7" s="3" t="inlineStr"/>
+      <c r="B7" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">PALMILHA       </t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">DIVA ROSADO (SEM DUB)                   </t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,2155</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" s="3" t="inlineStr">
         <is>
           <t>ML</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="68" customHeight="1">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+    <row r="8" ht="68" customHeight="1" s="4">
+      <c r="A8" s="3" t="inlineStr"/>
+      <c r="B8" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="E8" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO ==&gt;      </t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">.                                       </t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      7,0000</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="K8" s="3" t="inlineStr">
         <is>
           <t>PRS</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="68" customHeight="1">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+    <row r="9" ht="68" customHeight="1" s="4">
+      <c r="A9" s="3" t="inlineStr"/>
+      <c r="B9" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E9" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E9" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLADO         </t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLA SOFT NUDE/BEIRA NEW NATURAL        </t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,2795</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    173,0000</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K9" s="3" t="inlineStr">
         <is>
           <t>PLACA</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="68" customHeight="1">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+    <row r="10" ht="68" customHeight="1" s="4">
+      <c r="A10" s="3" t="inlineStr"/>
+      <c r="B10" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E10" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="E10" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" s="3" t="inlineStr">
         <is>
           <t>               </t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">ESP BANANINHA REF7960                   </t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      7,0000</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J10" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  7.570,0000</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K10" s="3" t="inlineStr">
         <is>
           <t>.pr</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="68" customHeight="1">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+    <row r="11" ht="68" customHeight="1" s="4">
+      <c r="A11" s="3" t="inlineStr"/>
+      <c r="B11" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E11" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="E11" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">CABEDAL        </t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC PRETO - TB                     </t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      1,0569</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    265,3800</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K11" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="68" customHeight="1">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
+    <row r="12" ht="68" customHeight="1" s="4">
+      <c r="A12" s="3" t="inlineStr"/>
+      <c r="B12" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E12" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="E12" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">COST. PALMILHA </t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NA COR                                  </t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0009</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0000</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K12" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="68" customHeight="1">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
+    <row r="13" ht="68" customHeight="1" s="4">
+      <c r="A13" s="3" t="inlineStr"/>
+      <c r="B13" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E13" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F13" t="n">
+      <c r="E13" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO          </t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC PRETO - TB                     </t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1985</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    265,3800</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="68" customHeight="1">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
+    <row r="14" ht="68" customHeight="1" s="4">
+      <c r="A14" s="3" t="inlineStr"/>
+      <c r="B14" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E14" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="E14" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO         </t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO SINT ROSADO                      </t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1659</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    256,6400</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K14" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="68" customHeight="1">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
+    <row r="15" ht="68" customHeight="1" s="4">
+      <c r="A15" s="3" t="inlineStr"/>
+      <c r="B15" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E15" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="E15" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F15" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">FORRO SILK     </t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SILK ROSADO                             </t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,4959</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    196,8900</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K15" s="3" t="inlineStr">
         <is>
           <t>ML.</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="68" customHeight="1">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
+    <row r="16" ht="68" customHeight="1" s="4">
+      <c r="A16" s="3" t="inlineStr"/>
+      <c r="B16" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E16" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F16" t="n">
+      <c r="E16" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F16" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">PALMILHA       </t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">DIVA ROSADO (SEM DUB)                   </t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,2748</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="J16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="K16" s="3" t="inlineStr">
         <is>
           <t>ML</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="68" customHeight="1">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
+    <row r="17" ht="68" customHeight="1" s="4">
+      <c r="A17" s="3" t="inlineStr"/>
+      <c r="B17" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E17" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="E17" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO ==&gt;      </t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H17" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">.                                       </t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I17" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      9,0000</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J17" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="K17" s="3" t="inlineStr">
         <is>
           <t>PRS</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="68" customHeight="1">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+    <row r="18" ht="68" customHeight="1" s="4">
+      <c r="A18" s="3" t="inlineStr"/>
+      <c r="B18" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E18" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F18" t="n">
+      <c r="E18" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F18" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLADO         </t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLA SOFT NUDE/BEIRA PRETA              </t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,3593</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="J18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    173,0000</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="K18" s="3" t="inlineStr">
         <is>
           <t>PLACA</t>
         </is>
       </c>
     </row>
-    <row r="19" ht="68" customHeight="1">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
+    <row r="19" ht="68" customHeight="1" s="4">
+      <c r="A19" s="3" t="inlineStr"/>
+      <c r="B19" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E19" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F19" t="n">
+      <c r="E19" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F19" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>               </t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">ESP BANANINHA REF7960                   </t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      9,0000</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  7.570,0000</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="K19" s="3" t="inlineStr">
         <is>
           <t>.pr</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="68" customHeight="1">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
+    <row r="20" ht="68" customHeight="1" s="4">
+      <c r="A20" s="3" t="inlineStr"/>
+      <c r="B20" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E20" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="E20" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F20" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">CABEDAL        </t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="H20" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC OFF WHITE - TB                 </t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,7009</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    464,8700</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="K20" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="68" customHeight="1">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
+    <row r="21" ht="68" customHeight="1" s="4">
+      <c r="A21" s="3" t="inlineStr"/>
+      <c r="B21" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E21" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F21" t="n">
+      <c r="E21" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F21" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">COST. PALMILHA </t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="H21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NA COR                                  </t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0006</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,0000</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="K21" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="68" customHeight="1">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
+    <row r="22" ht="68" customHeight="1" s="4">
+      <c r="A22" s="3" t="inlineStr"/>
+      <c r="B22" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E22" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F22" t="n">
+      <c r="E22" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F22" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO          </t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">NEW TOSC OFF WHITE - TB                 </t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1316</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    464,8700</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="K22" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="68" customHeight="1">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
+    <row r="23" ht="68" customHeight="1" s="4">
+      <c r="A23" s="3" t="inlineStr"/>
+      <c r="B23" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E23" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F23" t="n">
+      <c r="E23" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F23" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO         </t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H23" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AVESSO SINT ROSADO                      </t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1100</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="J23" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    256,6400</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="K23" s="3" t="inlineStr">
         <is>
           <t>M2</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="68" customHeight="1">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
+    <row r="24" ht="68" customHeight="1" s="4">
+      <c r="A24" s="3" t="inlineStr"/>
+      <c r="B24" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E24" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F24" t="n">
+      <c r="E24" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F24" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">FORRO SILK     </t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="H24" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SILK ROSADO                             </t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,3288</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="J24" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    196,8900</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="K24" s="3" t="inlineStr">
         <is>
           <t>ML.</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="68" customHeight="1">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+    <row r="25" ht="68" customHeight="1" s="4">
+      <c r="A25" s="3" t="inlineStr"/>
+      <c r="B25" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E25" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F25" t="n">
+      <c r="E25" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F25" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">PALMILHA       </t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">DIVA ROSADO (SEM DUB)                   </t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,1823</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K25" s="3" t="inlineStr">
         <is>
           <t>ML</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="68" customHeight="1">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
+    <row r="26" ht="68" customHeight="1" s="4">
+      <c r="A26" s="3" t="inlineStr"/>
+      <c r="B26" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E26" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="E26" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F26" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SALTO ==&gt;      </t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="H26" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">.                                       </t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      6,0000</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="J26" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  1.081,8800</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="K26" s="3" t="inlineStr">
         <is>
           <t>PRS</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="68" customHeight="1">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
+    <row r="27" ht="68" customHeight="1" s="4">
+      <c r="A27" s="3" t="inlineStr"/>
+      <c r="B27" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E27" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="E27" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F27" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLADO         </t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="H27" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">SOLA SOFT NUDE/BEIRA NEW NATURAL        </t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      0,2395</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="J27" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">    173,0000</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="K27" s="3" t="inlineStr">
         <is>
           <t>PLACA</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="68" customHeight="1">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="n">
-        <v>18807</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>14/02/2025</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
+    <row r="28" ht="68" customHeight="1" s="4">
+      <c r="A28" s="3" t="inlineStr"/>
+      <c r="B28" s="3" t="n">
+        <v>18807</v>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>14/02/2025</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E28" t="n">
-        <v>131290</v>
-      </c>
-      <c r="F28" t="n">
+      <c r="E28" s="3" t="n">
+        <v>131290</v>
+      </c>
+      <c r="F28" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" s="3" t="inlineStr">
         <is>
           <t>               </t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="H28" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">ESP BANANINHA REF7960                   </t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="I28" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">      6,0000</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">  7.570,0000</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="K28" s="3" t="inlineStr">
         <is>
           <t>.pr</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>